<commit_message>
updated qc overview, so that making plot files also adds to this overview automatically
</commit_message>
<xml_diff>
--- a/1_raw_files/STR23/221216_STR23_ctrl_OPT0024_opt0030_opt0424.xlsx
+++ b/1_raw_files/STR23/221216_STR23_ctrl_OPT0024_opt0030_opt0424.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mhuismans/surfdrive/Promotie/12. STRATEGIC/Analyse 2.0/1_raw_files/STR23/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC0AFA3-437D-8E48-831B-F9FE950BB944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="18975" windowHeight="11955"/>
+    <workbookView xWindow="120" yWindow="500" windowWidth="18980" windowHeight="11960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,8 +39,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,6 +77,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -117,7 +131,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -149,9 +163,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -183,6 +215,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -358,16 +408,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:Z17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:B17"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="2:26">
+    <row r="1" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -444,7 +494,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="2:26">
+    <row r="2" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B2">
         <v>21.1</v>
       </c>
@@ -521,7 +571,7 @@
         <v>2.3220000000000001</v>
       </c>
     </row>
-    <row r="3" spans="2:26">
+    <row r="3" spans="2:26" x14ac:dyDescent="0.2">
       <c r="C3">
         <v>2.3220000000000001</v>
       </c>
@@ -595,7 +645,7 @@
         <v>2.3220000000000001</v>
       </c>
     </row>
-    <row r="4" spans="2:26">
+    <row r="4" spans="2:26" x14ac:dyDescent="0.2">
       <c r="C4">
         <v>9.2870000000000008</v>
       </c>
@@ -669,7 +719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:26">
+    <row r="5" spans="2:26" x14ac:dyDescent="0.2">
       <c r="C5">
         <v>34.826999999999998</v>
       </c>
@@ -743,7 +793,7 @@
         <v>41.792999999999999</v>
       </c>
     </row>
-    <row r="6" spans="2:26">
+    <row r="6" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>1</v>
       </c>
@@ -820,84 +870,84 @@
         <v>14067.985000000001</v>
       </c>
     </row>
-    <row r="7" spans="2:26">
+    <row r="7" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>1</v>
       </c>
       <c r="C7">
-        <v>134.666</v>
+        <v>97.516999999999996</v>
       </c>
       <c r="D7">
-        <v>14873.661</v>
+        <v>17088.688999999998</v>
       </c>
       <c r="E7">
-        <v>18560.732</v>
+        <v>19006.523000000001</v>
       </c>
       <c r="F7">
-        <v>20919.715</v>
+        <v>12491.460999999999</v>
       </c>
       <c r="G7">
-        <v>16206.394</v>
+        <v>15298.557000000001</v>
       </c>
       <c r="H7">
-        <v>17367.311000000002</v>
+        <v>17968.664000000001</v>
       </c>
       <c r="I7">
-        <v>21261.023000000001</v>
+        <v>15830.257</v>
       </c>
       <c r="J7">
-        <v>16847.219000000001</v>
+        <v>20576.083999999999</v>
       </c>
       <c r="K7">
-        <v>34349.195</v>
+        <v>17153.701000000001</v>
       </c>
       <c r="L7">
-        <v>12514.68</v>
+        <v>16108.877</v>
       </c>
       <c r="M7">
-        <v>136.988</v>
+        <v>15516.81</v>
       </c>
       <c r="N7">
-        <v>97.516999999999996</v>
+        <v>15651.476000000001</v>
       </c>
       <c r="O7">
-        <v>109.126</v>
+        <v>19575.373</v>
       </c>
       <c r="P7">
-        <v>123.057</v>
+        <v>16317.842000000001</v>
       </c>
       <c r="Q7">
-        <v>99.838999999999999</v>
+        <v>16828.645</v>
       </c>
       <c r="R7">
-        <v>92.873000000000005</v>
+        <v>19094.754000000001</v>
       </c>
       <c r="S7">
-        <v>104.482</v>
+        <v>15149.96</v>
       </c>
       <c r="T7">
-        <v>123.057</v>
+        <v>14386.075999999999</v>
       </c>
       <c r="U7">
-        <v>130.023</v>
+        <v>16329.450999999999</v>
       </c>
       <c r="V7">
-        <v>90.551000000000002</v>
+        <v>12686.495000000001</v>
       </c>
       <c r="W7">
-        <v>85.908000000000001</v>
+        <v>12305.714</v>
       </c>
       <c r="X7">
-        <v>125.379</v>
+        <v>15073.339</v>
       </c>
       <c r="Y7">
-        <v>104.482</v>
+        <v>18005.813999999998</v>
       </c>
       <c r="Z7">
-        <v>106.804</v>
+        <v>18581.629000000001</v>
       </c>
     </row>
-    <row r="8" spans="2:26">
+    <row r="8" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>1</v>
       </c>
@@ -974,7 +1024,7 @@
         <v>18581.629000000001</v>
       </c>
     </row>
-    <row r="9" spans="2:26">
+    <row r="9" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>1</v>
       </c>
@@ -1051,7 +1101,7 @@
         <v>69.655000000000001</v>
       </c>
     </row>
-    <row r="10" spans="2:26">
+    <row r="10" spans="2:26" x14ac:dyDescent="0.2">
       <c r="C10">
         <v>39.470999999999997</v>
       </c>
@@ -1125,7 +1175,7 @@
         <v>23.218</v>
       </c>
     </row>
-    <row r="11" spans="2:26">
+    <row r="11" spans="2:26" x14ac:dyDescent="0.2">
       <c r="C11">
         <v>99.838999999999999</v>
       </c>
@@ -1199,7 +1249,7 @@
         <v>48.758000000000003</v>
       </c>
     </row>
-    <row r="12" spans="2:26">
+    <row r="12" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>2</v>
       </c>
@@ -1276,7 +1326,7 @@
         <v>6654.3729999999996</v>
       </c>
     </row>
-    <row r="13" spans="2:26">
+    <row r="13" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>2</v>
       </c>
@@ -1353,7 +1403,7 @@
         <v>5391.2960000000003</v>
       </c>
     </row>
-    <row r="14" spans="2:26">
+    <row r="14" spans="2:26" x14ac:dyDescent="0.2">
       <c r="C14">
         <v>60.368000000000002</v>
       </c>
@@ -1427,7 +1477,7 @@
         <v>23.218</v>
       </c>
     </row>
-    <row r="15" spans="2:26">
+    <row r="15" spans="2:26" x14ac:dyDescent="0.2">
       <c r="C15">
         <v>44.115000000000002</v>
       </c>
@@ -1501,7 +1551,7 @@
         <v>30.184000000000001</v>
       </c>
     </row>
-    <row r="16" spans="2:26">
+    <row r="16" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>3</v>
       </c>
@@ -1578,7 +1628,7 @@
         <v>1056.434</v>
       </c>
     </row>
-    <row r="17" spans="2:26">
+    <row r="17" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>3</v>
       </c>
@@ -1661,24 +1711,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>